<commit_message>
successful multichannel and irregular states
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valwur0b\Desktop\mindsphere\GCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8101AA-FE4B-4D91-A86C-3630FC4F65D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F836A4E6-97D6-46BA-95C4-D7284A515B85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{82EC0E01-F685-445B-A746-A0521EC60300}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'7h_Consumption'!$A$1:$E$287</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Anomalie_1!$A$1:$E$287</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Anomalie_2!$A$1:$E$287</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Normal!$A$1:$E$287</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Normal!$A$1:$E$290</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Too_long_1!$A$1:$E$287</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Too_long_2!$A$1:$E$287</definedName>
   </definedNames>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6040" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6048" uniqueCount="298">
   <si>
     <t>DATUM</t>
   </si>
@@ -935,6 +935,15 @@
   <si>
     <t>235119</t>
   </si>
+  <si>
+    <t>000236</t>
+  </si>
+  <si>
+    <t>000234</t>
+  </si>
+  <si>
+    <t>000235</t>
+  </si>
 </sst>
 </file>
 
@@ -943,7 +952,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -967,6 +976,12 @@
       <color rgb="FFFF0000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1356,10 +1371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581CE720-8407-422B-AE13-83C832889133}">
-  <dimension ref="A1:E287"/>
+  <dimension ref="A1:E290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="D258" sqref="D258"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,7 +1408,7 @@
         <v>44364</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>296</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -1401,7 +1416,7 @@
       <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2">
         <v>1</v>
       </c>
     </row>
@@ -1410,7 +1425,7 @@
         <v>44364</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -1418,7 +1433,7 @@
       <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3">
         <v>1</v>
       </c>
     </row>
@@ -1427,7 +1442,7 @@
         <v>44364</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>295</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -1435,8 +1450,8 @@
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3">
-        <v>0</v>
+      <c r="E4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1444,7 +1459,7 @@
         <v>44364</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
@@ -1461,7 +1476,7 @@
         <v>44364</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>6</v>
@@ -1478,7 +1493,7 @@
         <v>44364</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>6</v>
@@ -1495,7 +1510,7 @@
         <v>44364</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>6</v>
@@ -1512,7 +1527,7 @@
         <v>44364</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>6</v>
@@ -1529,7 +1544,7 @@
         <v>44364</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>6</v>
@@ -1546,7 +1561,7 @@
         <v>44364</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>6</v>
@@ -1563,7 +1578,7 @@
         <v>44364</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>6</v>
@@ -1580,7 +1595,7 @@
         <v>44364</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>6</v>
@@ -1597,7 +1612,7 @@
         <v>44364</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>6</v>
@@ -1614,7 +1629,7 @@
         <v>44364</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>6</v>
@@ -1631,7 +1646,7 @@
         <v>44364</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>6</v>
@@ -1648,7 +1663,7 @@
         <v>44364</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>6</v>
@@ -1665,7 +1680,7 @@
         <v>44364</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>6</v>
@@ -1682,7 +1697,7 @@
         <v>44364</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>6</v>
@@ -1699,7 +1714,7 @@
         <v>44364</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>6</v>
@@ -1716,7 +1731,7 @@
         <v>44364</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>6</v>
@@ -1733,7 +1748,7 @@
         <v>44364</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>6</v>
@@ -1750,7 +1765,7 @@
         <v>44364</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>6</v>
@@ -1767,7 +1782,7 @@
         <v>44364</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>6</v>
@@ -1784,7 +1799,7 @@
         <v>44364</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>6</v>
@@ -1801,7 +1816,7 @@
         <v>44364</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>6</v>
@@ -1818,7 +1833,7 @@
         <v>44364</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>6</v>
@@ -1835,7 +1850,7 @@
         <v>44364</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>6</v>
@@ -1852,7 +1867,7 @@
         <v>44364</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>6</v>
@@ -1869,7 +1884,7 @@
         <v>44364</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>6</v>
@@ -1886,7 +1901,7 @@
         <v>44364</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>6</v>
@@ -1903,7 +1918,7 @@
         <v>44364</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>6</v>
@@ -1920,7 +1935,7 @@
         <v>44364</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>6</v>
@@ -1937,7 +1952,7 @@
         <v>44364</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>6</v>
@@ -1954,7 +1969,7 @@
         <v>44364</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>6</v>
@@ -1971,7 +1986,7 @@
         <v>44364</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>6</v>
@@ -1988,7 +2003,7 @@
         <v>44364</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>6</v>
@@ -2005,7 +2020,7 @@
         <v>44364</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>6</v>
@@ -2022,7 +2037,7 @@
         <v>44364</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>6</v>
@@ -2039,7 +2054,7 @@
         <v>44364</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>6</v>
@@ -2056,7 +2071,7 @@
         <v>44364</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>6</v>
@@ -2073,7 +2088,7 @@
         <v>44364</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>6</v>
@@ -2090,7 +2105,7 @@
         <v>44364</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>6</v>
@@ -2107,7 +2122,7 @@
         <v>44364</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>6</v>
@@ -2124,7 +2139,7 @@
         <v>44364</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>6</v>
@@ -2141,7 +2156,7 @@
         <v>44364</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>6</v>
@@ -2158,7 +2173,7 @@
         <v>44364</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>6</v>
@@ -2175,7 +2190,7 @@
         <v>44364</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>6</v>
@@ -2192,7 +2207,7 @@
         <v>44364</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>6</v>
@@ -2209,7 +2224,7 @@
         <v>44364</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>6</v>
@@ -2226,7 +2241,7 @@
         <v>44364</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>6</v>
@@ -2243,7 +2258,7 @@
         <v>44364</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>6</v>
@@ -2260,7 +2275,7 @@
         <v>44364</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>6</v>
@@ -2277,7 +2292,7 @@
         <v>44364</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>6</v>
@@ -2294,7 +2309,7 @@
         <v>44364</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>6</v>
@@ -2311,7 +2326,7 @@
         <v>44364</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>6</v>
@@ -2328,7 +2343,7 @@
         <v>44364</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>6</v>
@@ -2345,7 +2360,7 @@
         <v>44364</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>6</v>
@@ -2362,7 +2377,7 @@
         <v>44364</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>6</v>
@@ -2379,7 +2394,7 @@
         <v>44364</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>6</v>
@@ -2396,7 +2411,7 @@
         <v>44364</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>6</v>
@@ -2413,7 +2428,7 @@
         <v>44364</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>6</v>
@@ -2430,7 +2445,7 @@
         <v>44364</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>6</v>
@@ -2447,7 +2462,7 @@
         <v>44364</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>6</v>
@@ -2464,7 +2479,7 @@
         <v>44364</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>6</v>
@@ -2481,7 +2496,7 @@
         <v>44364</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>6</v>
@@ -2498,7 +2513,7 @@
         <v>44364</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>6</v>
@@ -2515,7 +2530,7 @@
         <v>44364</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>6</v>
@@ -2532,7 +2547,7 @@
         <v>44364</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>6</v>
@@ -2549,7 +2564,7 @@
         <v>44364</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>6</v>
@@ -2566,7 +2581,7 @@
         <v>44364</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>6</v>
@@ -2583,7 +2598,7 @@
         <v>44364</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>6</v>
@@ -2600,7 +2615,7 @@
         <v>44364</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>6</v>
@@ -2617,7 +2632,7 @@
         <v>44364</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>6</v>
@@ -2634,7 +2649,7 @@
         <v>44364</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>6</v>
@@ -2651,7 +2666,7 @@
         <v>44364</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>6</v>
@@ -2668,7 +2683,7 @@
         <v>44364</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>6</v>
@@ -2685,7 +2700,7 @@
         <v>44364</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>6</v>
@@ -2702,7 +2717,7 @@
         <v>44364</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>6</v>
@@ -2719,7 +2734,7 @@
         <v>44364</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>6</v>
@@ -2736,7 +2751,7 @@
         <v>44364</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>6</v>
@@ -2753,7 +2768,7 @@
         <v>44364</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>6</v>
@@ -2770,7 +2785,7 @@
         <v>44364</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>6</v>
@@ -2787,7 +2802,7 @@
         <v>44364</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>6</v>
@@ -2804,7 +2819,7 @@
         <v>44364</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>6</v>
@@ -2821,7 +2836,7 @@
         <v>44364</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>6</v>
@@ -2838,7 +2853,7 @@
         <v>44364</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>6</v>
@@ -2855,7 +2870,7 @@
         <v>44364</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>6</v>
@@ -2872,7 +2887,7 @@
         <v>44364</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>6</v>
@@ -2889,7 +2904,7 @@
         <v>44364</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>6</v>
@@ -2906,7 +2921,7 @@
         <v>44364</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>6</v>
@@ -2923,7 +2938,7 @@
         <v>44364</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>6</v>
@@ -2940,7 +2955,7 @@
         <v>44364</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>6</v>
@@ -2957,7 +2972,7 @@
         <v>44364</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>6</v>
@@ -2974,7 +2989,7 @@
         <v>44364</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>6</v>
@@ -2991,7 +3006,7 @@
         <v>44364</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>6</v>
@@ -3008,16 +3023,16 @@
         <v>44364</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E97" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -3025,16 +3040,16 @@
         <v>44364</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E98" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -3042,7 +3057,7 @@
         <v>44364</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>6</v>
@@ -3059,7 +3074,7 @@
         <v>44364</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>6</v>
@@ -3076,7 +3091,7 @@
         <v>44364</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>6</v>
@@ -3093,7 +3108,7 @@
         <v>44364</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>6</v>
@@ -3110,7 +3125,7 @@
         <v>44364</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>6</v>
@@ -3127,7 +3142,7 @@
         <v>44364</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>6</v>
@@ -3144,7 +3159,7 @@
         <v>44364</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>6</v>
@@ -3161,7 +3176,7 @@
         <v>44364</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>6</v>
@@ -3178,7 +3193,7 @@
         <v>44364</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>6</v>
@@ -3195,7 +3210,7 @@
         <v>44364</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>6</v>
@@ -3212,7 +3227,7 @@
         <v>44364</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>6</v>
@@ -3229,7 +3244,7 @@
         <v>44364</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>6</v>
@@ -3246,7 +3261,7 @@
         <v>44364</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>6</v>
@@ -3263,7 +3278,7 @@
         <v>44364</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>6</v>
@@ -3280,7 +3295,7 @@
         <v>44364</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>6</v>
@@ -3297,7 +3312,7 @@
         <v>44364</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>6</v>
@@ -3314,7 +3329,7 @@
         <v>44364</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>6</v>
@@ -3331,7 +3346,7 @@
         <v>44364</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>6</v>
@@ -3348,7 +3363,7 @@
         <v>44364</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>6</v>
@@ -3365,7 +3380,7 @@
         <v>44364</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>6</v>
@@ -3382,7 +3397,7 @@
         <v>44364</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>6</v>
@@ -3399,7 +3414,7 @@
         <v>44364</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>6</v>
@@ -3416,7 +3431,7 @@
         <v>44364</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>6</v>
@@ -3433,7 +3448,7 @@
         <v>44364</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>6</v>
@@ -3450,7 +3465,7 @@
         <v>44364</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>6</v>
@@ -3467,7 +3482,7 @@
         <v>44364</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C124" s="3" t="s">
         <v>6</v>
@@ -3484,7 +3499,7 @@
         <v>44364</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>6</v>
@@ -3501,7 +3516,7 @@
         <v>44364</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>6</v>
@@ -3518,7 +3533,7 @@
         <v>44364</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>6</v>
@@ -3535,7 +3550,7 @@
         <v>44364</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>6</v>
@@ -3552,7 +3567,7 @@
         <v>44364</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>6</v>
@@ -3569,7 +3584,7 @@
         <v>44364</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>6</v>
@@ -3586,7 +3601,7 @@
         <v>44364</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>6</v>
@@ -3603,7 +3618,7 @@
         <v>44364</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>6</v>
@@ -3620,7 +3635,7 @@
         <v>44364</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>6</v>
@@ -3637,7 +3652,7 @@
         <v>44364</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>6</v>
@@ -3654,7 +3669,7 @@
         <v>44364</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C135" s="3" t="s">
         <v>6</v>
@@ -3671,7 +3686,7 @@
         <v>44364</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>6</v>
@@ -3688,7 +3703,7 @@
         <v>44364</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>6</v>
@@ -3705,7 +3720,7 @@
         <v>44364</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>6</v>
@@ -3722,7 +3737,7 @@
         <v>44364</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C139" s="3" t="s">
         <v>6</v>
@@ -3739,7 +3754,7 @@
         <v>44364</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C140" s="3" t="s">
         <v>6</v>
@@ -3756,7 +3771,7 @@
         <v>44364</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C141" s="3" t="s">
         <v>6</v>
@@ -3773,7 +3788,7 @@
         <v>44364</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C142" s="3" t="s">
         <v>6</v>
@@ -3790,7 +3805,7 @@
         <v>44364</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C143" s="3" t="s">
         <v>6</v>
@@ -3807,7 +3822,7 @@
         <v>44364</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C144" s="3" t="s">
         <v>6</v>
@@ -3824,7 +3839,7 @@
         <v>44364</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C145" s="3" t="s">
         <v>6</v>
@@ -3841,7 +3856,7 @@
         <v>44364</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C146" s="3" t="s">
         <v>6</v>
@@ -3858,7 +3873,7 @@
         <v>44364</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>6</v>
@@ -3875,7 +3890,7 @@
         <v>44364</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>6</v>
@@ -3892,7 +3907,7 @@
         <v>44364</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C149" s="3" t="s">
         <v>6</v>
@@ -3909,7 +3924,7 @@
         <v>44364</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>6</v>
@@ -3926,7 +3941,7 @@
         <v>44364</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C151" s="3" t="s">
         <v>6</v>
@@ -3943,7 +3958,7 @@
         <v>44364</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C152" s="3" t="s">
         <v>6</v>
@@ -3960,7 +3975,7 @@
         <v>44364</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>6</v>
@@ -3977,7 +3992,7 @@
         <v>44364</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>6</v>
@@ -3994,7 +4009,7 @@
         <v>44364</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>6</v>
@@ -4011,7 +4026,7 @@
         <v>44364</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>6</v>
@@ -4028,7 +4043,7 @@
         <v>44364</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C157" s="3" t="s">
         <v>6</v>
@@ -4045,33 +4060,33 @@
         <v>44364</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C158" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E158" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A159" s="4">
-        <v>44364</v>
-      </c>
-      <c r="B159" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="C159" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D159" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E159" s="5">
-        <v>0</v>
+      <c r="A159" s="2">
+        <v>44364</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E159" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -4079,13 +4094,13 @@
         <v>44364</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C160" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E160" s="3">
         <v>1</v>
@@ -4096,7 +4111,7 @@
         <v>44364</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C161" s="3" t="s">
         <v>6</v>
@@ -4109,19 +4124,19 @@
       </c>
     </row>
     <row r="162" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A162" s="2">
-        <v>44364</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D162" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E162" s="3">
+      <c r="A162" s="4">
+        <v>44364</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D162" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E162" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4130,7 +4145,7 @@
         <v>44364</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C163" s="3" t="s">
         <v>6</v>
@@ -4147,7 +4162,7 @@
         <v>44364</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C164" s="3" t="s">
         <v>6</v>
@@ -4164,7 +4179,7 @@
         <v>44364</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>6</v>
@@ -4181,7 +4196,7 @@
         <v>44364</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>6</v>
@@ -4198,7 +4213,7 @@
         <v>44364</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C167" s="3" t="s">
         <v>6</v>
@@ -4215,7 +4230,7 @@
         <v>44364</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C168" s="3" t="s">
         <v>6</v>
@@ -4232,7 +4247,7 @@
         <v>44364</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C169" s="3" t="s">
         <v>6</v>
@@ -4249,7 +4264,7 @@
         <v>44364</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C170" s="3" t="s">
         <v>6</v>
@@ -4266,7 +4281,7 @@
         <v>44364</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C171" s="3" t="s">
         <v>6</v>
@@ -4283,7 +4298,7 @@
         <v>44364</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C172" s="3" t="s">
         <v>6</v>
@@ -4300,7 +4315,7 @@
         <v>44364</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C173" s="3" t="s">
         <v>6</v>
@@ -4317,7 +4332,7 @@
         <v>44364</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C174" s="3" t="s">
         <v>6</v>
@@ -4334,7 +4349,7 @@
         <v>44364</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C175" s="3" t="s">
         <v>6</v>
@@ -4351,7 +4366,7 @@
         <v>44364</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>6</v>
@@ -4368,7 +4383,7 @@
         <v>44364</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C177" s="3" t="s">
         <v>6</v>
@@ -4385,7 +4400,7 @@
         <v>44364</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C178" s="3" t="s">
         <v>6</v>
@@ -4402,7 +4417,7 @@
         <v>44364</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C179" s="3" t="s">
         <v>6</v>
@@ -4419,7 +4434,7 @@
         <v>44364</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C180" s="3" t="s">
         <v>6</v>
@@ -4436,7 +4451,7 @@
         <v>44364</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C181" s="3" t="s">
         <v>6</v>
@@ -4453,7 +4468,7 @@
         <v>44364</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C182" s="3" t="s">
         <v>6</v>
@@ -4470,7 +4485,7 @@
         <v>44364</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C183" s="3" t="s">
         <v>6</v>
@@ -4487,7 +4502,7 @@
         <v>44364</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C184" s="3" t="s">
         <v>6</v>
@@ -4504,7 +4519,7 @@
         <v>44364</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>6</v>
@@ -4521,7 +4536,7 @@
         <v>44364</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C186" s="3" t="s">
         <v>6</v>
@@ -4538,7 +4553,7 @@
         <v>44364</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C187" s="3" t="s">
         <v>6</v>
@@ -4555,7 +4570,7 @@
         <v>44364</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C188" s="3" t="s">
         <v>6</v>
@@ -4572,7 +4587,7 @@
         <v>44364</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C189" s="3" t="s">
         <v>6</v>
@@ -4589,7 +4604,7 @@
         <v>44364</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C190" s="3" t="s">
         <v>6</v>
@@ -4606,7 +4621,7 @@
         <v>44364</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C191" s="3" t="s">
         <v>6</v>
@@ -4623,7 +4638,7 @@
         <v>44364</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C192" s="3" t="s">
         <v>6</v>
@@ -4640,7 +4655,7 @@
         <v>44364</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>6</v>
@@ -4657,7 +4672,7 @@
         <v>44364</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>6</v>
@@ -4674,7 +4689,7 @@
         <v>44364</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>6</v>
@@ -4691,7 +4706,7 @@
         <v>44364</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C196" s="3" t="s">
         <v>6</v>
@@ -4708,7 +4723,7 @@
         <v>44364</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C197" s="3" t="s">
         <v>6</v>
@@ -4725,7 +4740,7 @@
         <v>44364</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C198" s="3" t="s">
         <v>6</v>
@@ -4742,7 +4757,7 @@
         <v>44364</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C199" s="3" t="s">
         <v>6</v>
@@ -4759,7 +4774,7 @@
         <v>44364</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C200" s="3" t="s">
         <v>6</v>
@@ -4776,7 +4791,7 @@
         <v>44364</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C201" s="3" t="s">
         <v>6</v>
@@ -4793,7 +4808,7 @@
         <v>44364</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C202" s="3" t="s">
         <v>6</v>
@@ -4810,7 +4825,7 @@
         <v>44364</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C203" s="3" t="s">
         <v>6</v>
@@ -4827,7 +4842,7 @@
         <v>44364</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C204" s="3" t="s">
         <v>6</v>
@@ -4844,7 +4859,7 @@
         <v>44364</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C205" s="3" t="s">
         <v>6</v>
@@ -4861,7 +4876,7 @@
         <v>44364</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C206" s="3" t="s">
         <v>6</v>
@@ -4878,7 +4893,7 @@
         <v>44364</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C207" s="3" t="s">
         <v>6</v>
@@ -4895,7 +4910,7 @@
         <v>44364</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C208" s="3" t="s">
         <v>6</v>
@@ -4912,7 +4927,7 @@
         <v>44364</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C209" s="3" t="s">
         <v>6</v>
@@ -4929,7 +4944,7 @@
         <v>44364</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C210" s="3" t="s">
         <v>6</v>
@@ -4946,7 +4961,7 @@
         <v>44364</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C211" s="3" t="s">
         <v>6</v>
@@ -4963,7 +4978,7 @@
         <v>44364</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C212" s="3" t="s">
         <v>6</v>
@@ -4980,7 +4995,7 @@
         <v>44364</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C213" s="3" t="s">
         <v>6</v>
@@ -4997,7 +5012,7 @@
         <v>44364</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C214" s="3" t="s">
         <v>6</v>
@@ -5014,7 +5029,7 @@
         <v>44364</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C215" s="3" t="s">
         <v>6</v>
@@ -5031,7 +5046,7 @@
         <v>44364</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C216" s="3" t="s">
         <v>6</v>
@@ -5048,7 +5063,7 @@
         <v>44364</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C217" s="3" t="s">
         <v>6</v>
@@ -5065,7 +5080,7 @@
         <v>44364</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C218" s="3" t="s">
         <v>6</v>
@@ -5082,7 +5097,7 @@
         <v>44364</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C219" s="3" t="s">
         <v>6</v>
@@ -5099,7 +5114,7 @@
         <v>44364</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C220" s="3" t="s">
         <v>6</v>
@@ -5116,7 +5131,7 @@
         <v>44364</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C221" s="3" t="s">
         <v>6</v>
@@ -5133,7 +5148,7 @@
         <v>44364</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C222" s="3" t="s">
         <v>6</v>
@@ -5150,7 +5165,7 @@
         <v>44364</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>6</v>
@@ -5167,7 +5182,7 @@
         <v>44364</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C224" s="3" t="s">
         <v>6</v>
@@ -5184,7 +5199,7 @@
         <v>44364</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C225" s="3" t="s">
         <v>6</v>
@@ -5201,7 +5216,7 @@
         <v>44364</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C226" s="3" t="s">
         <v>6</v>
@@ -5218,7 +5233,7 @@
         <v>44364</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C227" s="3" t="s">
         <v>6</v>
@@ -5235,7 +5250,7 @@
         <v>44364</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C228" s="3" t="s">
         <v>6</v>
@@ -5252,7 +5267,7 @@
         <v>44364</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C229" s="3" t="s">
         <v>6</v>
@@ -5269,7 +5284,7 @@
         <v>44364</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C230" s="3" t="s">
         <v>6</v>
@@ -5286,7 +5301,7 @@
         <v>44364</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C231" s="3" t="s">
         <v>6</v>
@@ -5303,7 +5318,7 @@
         <v>44364</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C232" s="3" t="s">
         <v>6</v>
@@ -5320,7 +5335,7 @@
         <v>44364</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C233" s="3" t="s">
         <v>6</v>
@@ -5337,7 +5352,7 @@
         <v>44364</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C234" s="3" t="s">
         <v>6</v>
@@ -5354,7 +5369,7 @@
         <v>44364</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C235" s="3" t="s">
         <v>6</v>
@@ -5371,7 +5386,7 @@
         <v>44364</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C236" s="3" t="s">
         <v>6</v>
@@ -5388,7 +5403,7 @@
         <v>44364</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C237" s="3" t="s">
         <v>6</v>
@@ -5405,7 +5420,7 @@
         <v>44364</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C238" s="3" t="s">
         <v>6</v>
@@ -5422,7 +5437,7 @@
         <v>44364</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C239" s="3" t="s">
         <v>6</v>
@@ -5439,7 +5454,7 @@
         <v>44364</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C240" s="3" t="s">
         <v>6</v>
@@ -5456,7 +5471,7 @@
         <v>44364</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C241" s="3" t="s">
         <v>6</v>
@@ -5473,7 +5488,7 @@
         <v>44364</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C242" s="3" t="s">
         <v>6</v>
@@ -5490,7 +5505,7 @@
         <v>44364</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C243" s="3" t="s">
         <v>6</v>
@@ -5507,7 +5522,7 @@
         <v>44364</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C244" s="3" t="s">
         <v>6</v>
@@ -5524,7 +5539,7 @@
         <v>44364</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C245" s="3" t="s">
         <v>6</v>
@@ -5541,7 +5556,7 @@
         <v>44364</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C246" s="3" t="s">
         <v>6</v>
@@ -5558,7 +5573,7 @@
         <v>44364</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C247" s="3" t="s">
         <v>6</v>
@@ -5575,7 +5590,7 @@
         <v>44364</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C248" s="3" t="s">
         <v>6</v>
@@ -5592,7 +5607,7 @@
         <v>44364</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C249" s="3" t="s">
         <v>6</v>
@@ -5609,7 +5624,7 @@
         <v>44364</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C250" s="3" t="s">
         <v>6</v>
@@ -5626,7 +5641,7 @@
         <v>44364</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C251" s="3" t="s">
         <v>6</v>
@@ -5643,32 +5658,32 @@
         <v>44364</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C252" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D252" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E252" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="253" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A253" s="4">
-        <v>44364</v>
-      </c>
-      <c r="B253" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="C253" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D253" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E253" s="5">
+      <c r="A253" s="2">
+        <v>44364</v>
+      </c>
+      <c r="B253" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C253" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D253" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E253" s="3">
         <v>1</v>
       </c>
     </row>
@@ -5677,16 +5692,16 @@
         <v>44364</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C254" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D254" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E254" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="255" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -5694,7 +5709,7 @@
         <v>44364</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C255" s="3" t="s">
         <v>6</v>
@@ -5707,19 +5722,19 @@
       </c>
     </row>
     <row r="256" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A256" s="2">
-        <v>44364</v>
-      </c>
-      <c r="B256" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C256" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D256" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E256" s="3">
+      <c r="A256" s="4">
+        <v>44364</v>
+      </c>
+      <c r="B256" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C256" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D256" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E256" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5728,7 +5743,7 @@
         <v>44364</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C257" s="3" t="s">
         <v>6</v>
@@ -5745,7 +5760,7 @@
         <v>44364</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C258" s="3" t="s">
         <v>6</v>
@@ -5762,7 +5777,7 @@
         <v>44364</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C259" s="3" t="s">
         <v>6</v>
@@ -5779,7 +5794,7 @@
         <v>44364</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C260" s="3" t="s">
         <v>6</v>
@@ -5796,13 +5811,13 @@
         <v>44364</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C261" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D261" s="3" t="s">
-        <v>7</v>
+      <c r="D261" s="3">
+        <v>2</v>
       </c>
       <c r="E261" s="3">
         <v>1</v>
@@ -5813,7 +5828,7 @@
         <v>44364</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C262" s="3" t="s">
         <v>6</v>
@@ -5830,7 +5845,7 @@
         <v>44364</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C263" s="3" t="s">
         <v>6</v>
@@ -5847,7 +5862,7 @@
         <v>44364</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C264" s="3" t="s">
         <v>6</v>
@@ -5864,7 +5879,7 @@
         <v>44364</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C265" s="3" t="s">
         <v>6</v>
@@ -5881,7 +5896,7 @@
         <v>44364</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C266" s="3" t="s">
         <v>6</v>
@@ -5898,7 +5913,7 @@
         <v>44364</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C267" s="3" t="s">
         <v>6</v>
@@ -5915,7 +5930,7 @@
         <v>44364</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C268" s="3" t="s">
         <v>6</v>
@@ -5932,7 +5947,7 @@
         <v>44364</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C269" s="3" t="s">
         <v>6</v>
@@ -5949,7 +5964,7 @@
         <v>44364</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C270" s="3" t="s">
         <v>6</v>
@@ -5966,7 +5981,7 @@
         <v>44364</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C271" s="3" t="s">
         <v>6</v>
@@ -5983,7 +5998,7 @@
         <v>44364</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C272" s="3" t="s">
         <v>6</v>
@@ -6000,7 +6015,7 @@
         <v>44364</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C273" s="3" t="s">
         <v>6</v>
@@ -6017,7 +6032,7 @@
         <v>44364</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C274" s="3" t="s">
         <v>6</v>
@@ -6034,7 +6049,7 @@
         <v>44364</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C275" s="3" t="s">
         <v>6</v>
@@ -6051,7 +6066,7 @@
         <v>44364</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C276" s="3" t="s">
         <v>6</v>
@@ -6068,7 +6083,7 @@
         <v>44364</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C277" s="3" t="s">
         <v>6</v>
@@ -6085,7 +6100,7 @@
         <v>44364</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C278" s="3" t="s">
         <v>6</v>
@@ -6102,7 +6117,7 @@
         <v>44364</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C279" s="3" t="s">
         <v>6</v>
@@ -6119,7 +6134,7 @@
         <v>44364</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C280" s="3" t="s">
         <v>6</v>
@@ -6136,7 +6151,7 @@
         <v>44364</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C281" s="3" t="s">
         <v>6</v>
@@ -6153,7 +6168,7 @@
         <v>44364</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C282" s="3" t="s">
         <v>6</v>
@@ -6170,7 +6185,7 @@
         <v>44364</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C283" s="3" t="s">
         <v>6</v>
@@ -6187,7 +6202,7 @@
         <v>44364</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C284" s="3" t="s">
         <v>6</v>
@@ -6204,7 +6219,7 @@
         <v>44364</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C285" s="3" t="s">
         <v>6</v>
@@ -6221,7 +6236,7 @@
         <v>44364</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C286" s="3" t="s">
         <v>6</v>
@@ -6238,15 +6253,66 @@
         <v>44364</v>
       </c>
       <c r="B287" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C287" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D287" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E287" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A288" s="2">
+        <v>44364</v>
+      </c>
+      <c r="B288" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C288" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D288" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E288" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A289" s="2">
+        <v>44364</v>
+      </c>
+      <c r="B289" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C289" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D289" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E289" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A290" s="2">
+        <v>44364</v>
+      </c>
+      <c r="B290" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="C287" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D287" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E287" s="3">
+      <c r="C290" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D290" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E290" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6256,6 +6322,7 @@
       <sortCondition ref="B1:B287"/>
     </sortState>
   </autoFilter>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
@@ -20993,7 +21060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5AC9E73-68EE-4C2A-95A4-9C48DF7641DC}">
   <dimension ref="A1:E287"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="E219" sqref="E219"/>
     </sheetView>
   </sheetViews>
@@ -30806,11 +30873,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D29DC643-CCE3-4B45-976A-815C18F87E3B}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E287"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E264" sqref="E264"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30856,7 +30922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44364</v>
       </c>
@@ -30873,7 +30939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44364</v>
       </c>
@@ -30907,7 +30973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44364</v>
       </c>
@@ -30924,7 +30990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44364</v>
       </c>
@@ -30958,7 +31024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44364</v>
       </c>
@@ -30975,7 +31041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44364</v>
       </c>
@@ -31009,7 +31075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44364</v>
       </c>
@@ -31026,7 +31092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44364</v>
       </c>
@@ -31060,7 +31126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44364</v>
       </c>
@@ -31077,7 +31143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44364</v>
       </c>
@@ -31111,7 +31177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44364</v>
       </c>
@@ -31128,7 +31194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44364</v>
       </c>
@@ -31162,7 +31228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44364</v>
       </c>
@@ -31179,7 +31245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44364</v>
       </c>
@@ -31213,7 +31279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44364</v>
       </c>
@@ -31230,7 +31296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44364</v>
       </c>
@@ -31264,7 +31330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44364</v>
       </c>
@@ -31281,7 +31347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44364</v>
       </c>
@@ -31315,7 +31381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44364</v>
       </c>
@@ -31332,7 +31398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44364</v>
       </c>
@@ -31366,7 +31432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44364</v>
       </c>
@@ -31383,7 +31449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>44364</v>
       </c>
@@ -31417,7 +31483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>44364</v>
       </c>
@@ -31434,7 +31500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>44364</v>
       </c>
@@ -31468,7 +31534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>44364</v>
       </c>
@@ -31485,7 +31551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>44364</v>
       </c>
@@ -31519,7 +31585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>44364</v>
       </c>
@@ -31536,7 +31602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>44364</v>
       </c>
@@ -31570,7 +31636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44364</v>
       </c>
@@ -31587,7 +31653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>44364</v>
       </c>
@@ -31621,7 +31687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>44364</v>
       </c>
@@ -31638,7 +31704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>44364</v>
       </c>
@@ -31672,7 +31738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>44364</v>
       </c>
@@ -31689,7 +31755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>44364</v>
       </c>
@@ -31723,7 +31789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>44364</v>
       </c>
@@ -31740,7 +31806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>44364</v>
       </c>
@@ -31774,7 +31840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>44364</v>
       </c>
@@ -31791,7 +31857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>44364</v>
       </c>
@@ -31825,7 +31891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>44364</v>
       </c>
@@ -31842,7 +31908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>44364</v>
       </c>
@@ -31876,7 +31942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>44364</v>
       </c>
@@ -31893,7 +31959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>44364</v>
       </c>
@@ -31927,7 +31993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>44364</v>
       </c>
@@ -31944,7 +32010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>44364</v>
       </c>
@@ -31978,7 +32044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>44364</v>
       </c>
@@ -31995,7 +32061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>44364</v>
       </c>
@@ -32029,7 +32095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>44364</v>
       </c>
@@ -32046,7 +32112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>44364</v>
       </c>
@@ -32080,7 +32146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>44364</v>
       </c>
@@ -32097,7 +32163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>44364</v>
       </c>
@@ -32131,7 +32197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>44364</v>
       </c>
@@ -32148,7 +32214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>44364</v>
       </c>
@@ -32182,7 +32248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>44364</v>
       </c>
@@ -32199,7 +32265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>44364</v>
       </c>
@@ -32233,7 +32299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>44364</v>
       </c>
@@ -32250,7 +32316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>44364</v>
       </c>
@@ -32284,7 +32350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>44364</v>
       </c>
@@ -32301,7 +32367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>44364</v>
       </c>
@@ -32335,7 +32401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>44364</v>
       </c>
@@ -32352,7 +32418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>44364</v>
       </c>
@@ -32386,7 +32452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>44364</v>
       </c>
@@ -32403,7 +32469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>44364</v>
       </c>
@@ -32437,7 +32503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>44364</v>
       </c>
@@ -32471,7 +32537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>44364</v>
       </c>
@@ -32488,7 +32554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>44364</v>
       </c>
@@ -32522,7 +32588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>44364</v>
       </c>
@@ -32539,7 +32605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>44364</v>
       </c>
@@ -32573,7 +32639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>44364</v>
       </c>
@@ -32590,7 +32656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>44364</v>
       </c>
@@ -32624,7 +32690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>44364</v>
       </c>
@@ -32641,7 +32707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>44364</v>
       </c>
@@ -32675,7 +32741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>44364</v>
       </c>
@@ -32692,7 +32758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>44364</v>
       </c>
@@ -32726,7 +32792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>44364</v>
       </c>
@@ -32743,7 +32809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>44364</v>
       </c>
@@ -32777,7 +32843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>44364</v>
       </c>
@@ -32794,7 +32860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>44364</v>
       </c>
@@ -32828,7 +32894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>44364</v>
       </c>
@@ -32845,7 +32911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>44364</v>
       </c>
@@ -32879,7 +32945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>44364</v>
       </c>
@@ -32896,7 +32962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>44364</v>
       </c>
@@ -32930,7 +32996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>44364</v>
       </c>
@@ -32947,7 +33013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>44364</v>
       </c>
@@ -32981,7 +33047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>44364</v>
       </c>
@@ -32998,7 +33064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>44364</v>
       </c>
@@ -33032,7 +33098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>44364</v>
       </c>
@@ -33049,7 +33115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>44364</v>
       </c>
@@ -33083,7 +33149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>44364</v>
       </c>
@@ -33100,7 +33166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>44364</v>
       </c>
@@ -33134,7 +33200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>44364</v>
       </c>
@@ -33151,7 +33217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>44364</v>
       </c>
@@ -33185,7 +33251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>44364</v>
       </c>
@@ -33202,7 +33268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>44364</v>
       </c>
@@ -33236,7 +33302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>44364</v>
       </c>
@@ -33253,7 +33319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>44364</v>
       </c>
@@ -33287,7 +33353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>44364</v>
       </c>
@@ -33304,7 +33370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>44364</v>
       </c>
@@ -33338,7 +33404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>44364</v>
       </c>
@@ -33355,7 +33421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>44364</v>
       </c>
@@ -33389,7 +33455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>44364</v>
       </c>
@@ -33406,7 +33472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>44364</v>
       </c>
@@ -33440,7 +33506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>44364</v>
       </c>
@@ -33457,7 +33523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>44364</v>
       </c>
@@ -33508,7 +33574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>44364</v>
       </c>
@@ -33525,7 +33591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>44364</v>
       </c>
@@ -33559,7 +33625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>44364</v>
       </c>
@@ -33576,7 +33642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>44364</v>
       </c>
@@ -33610,7 +33676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>44364</v>
       </c>
@@ -33627,7 +33693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>44364</v>
       </c>
@@ -33661,7 +33727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>44364</v>
       </c>
@@ -33678,7 +33744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>44364</v>
       </c>
@@ -33712,7 +33778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>44364</v>
       </c>
@@ -33729,7 +33795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>44364</v>
       </c>
@@ -33763,7 +33829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>44364</v>
       </c>
@@ -33780,7 +33846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>44364</v>
       </c>
@@ -33814,7 +33880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>44364</v>
       </c>
@@ -33831,7 +33897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>44364</v>
       </c>
@@ -33865,7 +33931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>44364</v>
       </c>
@@ -33882,7 +33948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>44364</v>
       </c>
@@ -33916,7 +33982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>44364</v>
       </c>
@@ -33933,7 +33999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>44364</v>
       </c>
@@ -33967,7 +34033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>44364</v>
       </c>
@@ -33984,7 +34050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>44364</v>
       </c>
@@ -34018,7 +34084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>44364</v>
       </c>
@@ -34035,7 +34101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>44364</v>
       </c>
@@ -34069,7 +34135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>44364</v>
       </c>
@@ -34086,7 +34152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>44364</v>
       </c>
@@ -34120,7 +34186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>44364</v>
       </c>
@@ -34137,7 +34203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>44364</v>
       </c>
@@ -34171,7 +34237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>44364</v>
       </c>
@@ -34188,7 +34254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>44364</v>
       </c>
@@ -34222,7 +34288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>44364</v>
       </c>
@@ -34239,7 +34305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>44364</v>
       </c>
@@ -34273,7 +34339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>44364</v>
       </c>
@@ -34290,7 +34356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>44364</v>
       </c>
@@ -34324,7 +34390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>44364</v>
       </c>
@@ -34341,7 +34407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>44364</v>
       </c>
@@ -34375,7 +34441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>44364</v>
       </c>
@@ -34392,7 +34458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>44364</v>
       </c>
@@ -34426,7 +34492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>44364</v>
       </c>
@@ -34443,7 +34509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>44364</v>
       </c>
@@ -34477,7 +34543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>44364</v>
       </c>
@@ -34494,7 +34560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>44364</v>
       </c>
@@ -34528,7 +34594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>44364</v>
       </c>
@@ -34545,7 +34611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>44364</v>
       </c>
@@ -34579,7 +34645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>44364</v>
       </c>
@@ -34596,7 +34662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>44364</v>
       </c>
@@ -34630,7 +34696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>44364</v>
       </c>
@@ -34647,7 +34713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>44364</v>
       </c>
@@ -34681,7 +34747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <v>44364</v>
       </c>
@@ -34698,7 +34764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>44364</v>
       </c>
@@ -34732,7 +34798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
         <v>44364</v>
       </c>
@@ -34749,7 +34815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
         <v>44364</v>
       </c>
@@ -34783,7 +34849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
         <v>44364</v>
       </c>
@@ -34800,7 +34866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
         <v>44364</v>
       </c>
@@ -34834,7 +34900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
         <v>44364</v>
       </c>
@@ -34851,7 +34917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
         <v>44364</v>
       </c>
@@ -34885,7 +34951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
         <v>44364</v>
       </c>
@@ -34902,7 +34968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
         <v>44364</v>
       </c>
@@ -34936,7 +35002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
         <v>44364</v>
       </c>
@@ -34953,7 +35019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
         <v>44364</v>
       </c>
@@ -34987,7 +35053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
         <v>44364</v>
       </c>
@@ -35004,7 +35070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
         <v>44364</v>
       </c>
@@ -35038,7 +35104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A249" s="2">
         <v>44364</v>
       </c>
@@ -35055,7 +35121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
         <v>44364</v>
       </c>
@@ -35106,7 +35172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A253" s="2">
         <v>44364</v>
       </c>
@@ -35123,7 +35189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A254" s="2">
         <v>44364</v>
       </c>
@@ -35157,7 +35223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A256" s="2">
         <v>44364</v>
       </c>
@@ -35174,7 +35240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A257" s="2">
         <v>44364</v>
       </c>
@@ -35208,7 +35274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A259" s="2">
         <v>44364</v>
       </c>
@@ -35225,7 +35291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A260" s="2">
         <v>44364</v>
       </c>
@@ -35259,7 +35325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A262" s="2">
         <v>44364</v>
       </c>
@@ -35276,7 +35342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A263" s="2">
         <v>44364</v>
       </c>
@@ -35310,7 +35376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A265" s="2">
         <v>44364</v>
       </c>
@@ -35327,7 +35393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A266" s="2">
         <v>44364</v>
       </c>
@@ -35361,7 +35427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A268" s="2">
         <v>44364</v>
       </c>
@@ -35378,7 +35444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A269" s="2">
         <v>44364</v>
       </c>
@@ -35412,7 +35478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A271" s="2">
         <v>44364</v>
       </c>
@@ -35429,7 +35495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A272" s="2">
         <v>44364</v>
       </c>
@@ -35463,7 +35529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A274" s="2">
         <v>44364</v>
       </c>
@@ -35480,7 +35546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A275" s="2">
         <v>44364</v>
       </c>
@@ -35514,7 +35580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A277" s="2">
         <v>44364</v>
       </c>
@@ -35531,7 +35597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A278" s="2">
         <v>44364</v>
       </c>
@@ -35565,7 +35631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A280" s="2">
         <v>44364</v>
       </c>
@@ -35582,7 +35648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A281" s="2">
         <v>44364</v>
       </c>
@@ -35616,7 +35682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A283" s="2">
         <v>44364</v>
       </c>
@@ -35633,7 +35699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A284" s="2">
         <v>44364</v>
       </c>
@@ -35667,7 +35733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A286" s="2">
         <v>44364</v>
       </c>
@@ -35684,7 +35750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A287" s="2">
         <v>44364</v>
       </c>
@@ -35703,11 +35769,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E287" xr:uid="{DC3B5614-AEF6-4C88-AB10-2BD7A30CCD33}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="2"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:E286">
       <sortCondition ref="B1:B287"/>
     </sortState>

</xml_diff>